<commit_message>
forgot to commit the comparison between MER and GP
</commit_message>
<xml_diff>
--- a/output/traffic_vergelijking.xlsx
+++ b/output/traffic_vergelijking.xlsx
@@ -1,43 +1,110 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Wouter SD/Addendum gp2019/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2709B0B0-2BF9-944C-86B9-D9CC3D7F4B2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DEN" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DEN" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>prognose</t>
+  </si>
+  <si>
+    <t>landingen</t>
+  </si>
+  <si>
+    <t>starts</t>
+  </si>
+  <si>
+    <t>totaal</t>
+  </si>
+  <si>
+    <t>dag 07-19 uur</t>
+  </si>
+  <si>
+    <t>avond 19-23 uur</t>
+  </si>
+  <si>
+    <t>nacht 23-06 uur</t>
+  </si>
+  <si>
+    <t>vroege ochtend 06-07 uur</t>
+  </si>
+  <si>
+    <t>MER</t>
+  </si>
+  <si>
+    <t>Verschil</t>
+  </si>
+  <si>
+    <t>GP2018</t>
+  </si>
+  <si>
+    <t>GP2019</t>
+  </si>
+  <si>
+    <t>Realisatie 2018</t>
+  </si>
+  <si>
+    <t>nacht</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,54 +113,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -381,194 +441,427 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>prognose</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr"/>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>landingen</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>starts</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>totaal</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>landingen</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>starts</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>totaal</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>dag 07-19 uur</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>174900</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>187300</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>362100</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>173600</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>188400</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>362000</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>avond 19-23 uur</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+      <c r="H4">
+        <f>B4-E4</f>
+        <v>1300</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:K4" si="0">C4-F4</f>
+        <v>-1100</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>52200</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>49900</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>102000</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>54800</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>51300</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>106000</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>nacht 23-06 uur</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+      <c r="H5">
+        <f t="shared" ref="H5:H8" si="1">B5-E5</f>
+        <v>-2600</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I8" si="2">C5-F5</f>
+        <v>-1400</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J8" si="3">D5-G5</f>
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>12700</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>4000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>16700</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>12400</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>4500</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>16900</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>vroege ochtend 06-07 uur</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>8200</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>7000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>15100</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>9200</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>5900</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>15100</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>totaal</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUM(B6:B7)</f>
+        <v>20900</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:J8" si="4">SUM(C6:C7)</f>
+        <v>11000</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="4"/>
+        <v>31800</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>21600</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>10400</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>32000</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>-700</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>600</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
         <v>247900</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C9">
         <v>248100</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D9">
         <v>496000</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E9">
         <v>249900</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F9">
         <v>250100</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G9">
         <v>500000</v>
+      </c>
+      <c r="H9">
+        <f>B9-E9</f>
+        <v>-2000</v>
+      </c>
+      <c r="I9">
+        <f>C9-F9</f>
+        <v>-2000</v>
+      </c>
+      <c r="J9">
+        <f>D9-G9</f>
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="3">
+        <v>172500</v>
+      </c>
+      <c r="C11" s="3">
+        <v>187900</v>
+      </c>
+      <c r="D11" s="3">
+        <v>360400</v>
+      </c>
+      <c r="E11" s="3">
+        <v>175500</v>
+      </c>
+      <c r="F11" s="3">
+        <v>184400</v>
+      </c>
+      <c r="G11" s="3">
+        <v>359800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>53600</v>
+      </c>
+      <c r="C12" s="3">
+        <v>50800</v>
+      </c>
+      <c r="D12" s="3">
+        <v>104500</v>
+      </c>
+      <c r="E12" s="3">
+        <v>51600</v>
+      </c>
+      <c r="F12" s="3">
+        <v>54800</v>
+      </c>
+      <c r="G12" s="3">
+        <v>106400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
+        <v>12300</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4100</v>
+      </c>
+      <c r="D13" s="3">
+        <v>16400</v>
+      </c>
+      <c r="E13" s="3">
+        <v>15400</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4700</v>
+      </c>
+      <c r="G13" s="3">
+        <v>20200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="3">
+        <v>9500</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5800</v>
+      </c>
+      <c r="D14" s="3">
+        <v>15300</v>
+      </c>
+      <c r="E14" s="3">
+        <v>6200</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4800</v>
+      </c>
+      <c r="G14" s="3">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B13:B14)</f>
+        <v>21800</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:G15" si="5">SUM(C13:C14)</f>
+        <v>9900</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="5"/>
+        <v>31700</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="5"/>
+        <v>21600</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="5"/>
+        <v>9500</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>31200</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="3">
+        <v>248000</v>
+      </c>
+      <c r="C17" s="3">
+        <v>248600</v>
+      </c>
+      <c r="D17" s="3">
+        <v>496600</v>
+      </c>
+      <c r="E17" s="3">
+        <v>248700</v>
+      </c>
+      <c r="F17" s="3">
+        <v>248800</v>
+      </c>
+      <c r="G17" s="3">
+        <v>497400</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:G1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <conditionalFormatting sqref="H3:J7 H9:J9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>